<commit_message>
Implementing ReportNG, adding listeners, capturing screenshots
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -33,10 +33,10 @@
     <t>postcode</t>
   </si>
   <si>
+    <t>alerttext</t>
+  </si>
+  <si>
     <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>alerttext</t>
   </si>
 </sst>
 </file>
@@ -372,10 +372,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -388,7 +391,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -402,7 +405,7 @@
         <v>123123</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating common Data Provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Ivan</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>Ivan Ivanov</t>
   </si>
 </sst>
 </file>
@@ -371,7 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -415,12 +427,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding parameterization, creating third test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Ivan</t>
   </si>
@@ -49,6 +49,36 @@
   </si>
   <si>
     <t>Ivan Ivanov</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Petya</t>
+  </si>
+  <si>
+    <t>Petrov</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>Sidor</t>
+  </si>
+  <si>
+    <t>Sidorov</t>
+  </si>
+  <si>
+    <t>sdsagg4</t>
+  </si>
+  <si>
+    <t>Kirill</t>
+  </si>
+  <si>
+    <t>Kirillov</t>
+  </si>
+  <si>
+    <t>sdfgre34</t>
   </si>
 </sst>
 </file>
@@ -381,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,6 +450,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -427,31 +499,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting up run modes for Test Data, implementing hashtable
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Ivan</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,7 +446,7 @@
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -456,8 +459,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,8 +476,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -484,8 +493,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -498,8 +510,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -511,6 +526,9 @@
       </c>
       <c r="D5" t="s">
         <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -563,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -601,7 +619,7 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>